<commit_message>
[fix] Battle Protocol design
</commit_message>
<xml_diff>
--- a/documents/WebAPI/プロトコル設計.xlsx
+++ b/documents/WebAPI/プロトコル設計.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\student\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\student\git\Sprout.git\documents\WebAPI\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="27">
   <si>
     <t>リソースのURI</t>
     <phoneticPr fontId="1"/>
@@ -99,32 +99,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>roomId1=123</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>roomId2=132</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>battleId=001</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>バトルの作成</t>
-    <rPh sb="4" eb="6">
-      <t>サクセイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>バトルの削除</t>
-    <rPh sb="4" eb="6">
-      <t>サクジョ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>http://nitta-lab-www2.is.konan-u.ac.jp/Sprout/Battles</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -161,14 +135,6 @@
   </si>
   <si>
     <t>http://nitta-lab-www2.is.konan-u.ac.jp/Sprout/Battles/{battleId}/Time</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>{
- "battleId":"1234",
- "teamId1":"123",
- "teamId2":"132"
-}</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -228,28 +194,11 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>勝敗情報の更新</t>
-    <rPh sb="0" eb="2">
-      <t>ショウハイ</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>ジョウホウ</t>
-    </rPh>
-    <rPh sb="5" eb="7">
-      <t>コウシン</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>type=team</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>type=team</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>type=result</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -685,8 +634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:A13"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -729,30 +678,20 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="8" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="67.5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="9"/>
-      <c r="B3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B3" s="2"/>
+      <c r="C3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>24</v>
-      </c>
+      <c r="F3" s="6"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="9"/>
@@ -763,19 +702,14 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" s="9"/>
-      <c r="B5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="B5" s="2"/>
+      <c r="C5" s="4" t="s">
         <v>5</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" s="8" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="4" t="s">
@@ -805,19 +739,19 @@
     </row>
     <row r="10" spans="1:9" ht="243" x14ac:dyDescent="0.15">
       <c r="A10" s="8" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
         <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.15">
@@ -830,37 +764,37 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A12" s="8"/>
       <c r="B12" s="2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A13" s="8"/>
       <c r="B13" s="2"/>
-      <c r="C13" t="s">
+      <c r="C13" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A14" s="8" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C14" t="s">
         <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.15">
@@ -872,14 +806,9 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A16" s="8"/>
-      <c r="B16" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="B16" s="2"/>
+      <c r="C16" s="4" t="s">
         <v>4</v>
-      </c>
-      <c r="D16" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
@@ -891,16 +820,16 @@
     </row>
     <row r="18" spans="1:4" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A18" s="8" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C18" t="s">
         <v>2</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">

</xml_diff>